<commit_message>
🥸fuzzy update, hapus file tidak penting
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,50 +441,42 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pelayanan</t>
+          <t>PELAYANAN</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Harga</t>
+          <t>HARGA</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Keputusan Fuzzy</t>
+          <t>SKOR_KELAYAKAN</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Derajat Keanggotaan</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Nilai Defuzzifikasi</t>
+          <t>KETERANGAN</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="B2" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="n">
-        <v>34513</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>100</v>
+        <v>22360</v>
+      </c>
+      <c r="D2" t="n">
+        <v>92</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Sangat Layak</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -497,60 +489,51 @@
       <c r="C3" t="n">
         <v>22012</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>100</v>
+      <c r="D3" t="n">
+        <v>89</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Sangat Layak</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="B4" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" t="n">
-        <v>22360</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>100</v>
+        <v>34513</v>
+      </c>
+      <c r="D4" t="n">
+        <v>87.50000000000001</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sangat Layak</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C5" t="n">
-        <v>20052</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>100</v>
+        <v>27315</v>
+      </c>
+      <c r="D5" t="n">
+        <v>86</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sangat Layak</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -563,126 +546,13 @@
       <c r="C6" t="n">
         <v>29811</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>78</v>
-      </c>
-      <c r="B7" t="n">
-        <v>86</v>
-      </c>
-      <c r="C7" t="n">
-        <v>27315</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>69</v>
-      </c>
-      <c r="B8" t="n">
-        <v>85</v>
-      </c>
-      <c r="C8" t="n">
-        <v>24551</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>88</v>
-      </c>
-      <c r="B9" t="n">
-        <v>100</v>
-      </c>
-      <c r="C9" t="n">
-        <v>35304</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0.9696</v>
-      </c>
-      <c r="F9" t="n">
-        <v>99.24000000000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>13</v>
-      </c>
-      <c r="B10" t="n">
-        <v>79</v>
-      </c>
-      <c r="C10" t="n">
-        <v>35119</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="F10" t="n">
-        <v>97.90730611447547</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>23</v>
-      </c>
-      <c r="B11" t="n">
-        <v>77</v>
-      </c>
-      <c r="C11" t="n">
-        <v>22825</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>sangat_layak</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="F11" t="n">
-        <v>96.25</v>
+      <c r="D6" t="n">
+        <v>85.2400728182956</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sangat Layak</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>